<commit_message>
feat: redacted work inform
</commit_message>
<xml_diff>
--- a/Punto1/Tablas resumen resultados.xlsx
+++ b/Punto1/Tablas resumen resultados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Semestre 08\Bases de Datos II\Proyectos\BD2-T4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Semestre 08\Bases de Datos II\Proyectos\BD2-T4\Punto1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE9C8A1-3A95-438D-B71F-6B42DEB3B39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C29C84-1167-4D24-901B-C12EB04592B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,16 +90,16 @@
     <t>Time (s)</t>
   </si>
   <si>
-    <t>Consulta 1</t>
-  </si>
-  <si>
-    <t>Consulta 2</t>
-  </si>
-  <si>
-    <t>Consulta 3</t>
-  </si>
-  <si>
-    <t>Consulta 4</t>
+    <t>Consulta D</t>
+  </si>
+  <si>
+    <t>Consulta C</t>
+  </si>
+  <si>
+    <t>Consulta B</t>
+  </si>
+  <si>
+    <t>Consulta A</t>
   </si>
 </sst>
 </file>
@@ -107,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -363,13 +363,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -384,16 +384,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -404,30 +428,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2ACDED-A748-4842-AE64-B04F60BB7257}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -737,23 +737,23 @@
   <sheetData>
     <row r="1" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="19" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="22" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="20"/>
-      <c r="I2" s="22"/>
+      <c r="I2" s="21"/>
       <c r="J2" s="20" t="s">
         <v>3</v>
       </c>
@@ -761,55 +761,55 @@
       <c r="L2" s="20"/>
       <c r="M2" s="20"/>
       <c r="N2" s="20"/>
-      <c r="O2" s="22"/>
+      <c r="O2" s="21"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="24" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="N3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="26" t="s">
+      <c r="O3" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="2">
         <v>100</v>
       </c>
@@ -857,7 +857,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="2">
         <v>1000</v>
       </c>
@@ -905,7 +905,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="2">
         <v>5000</v>
       </c>
@@ -953,7 +953,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="2">
         <v>10000</v>
       </c>
@@ -1001,7 +1001,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="18"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="9">
         <v>15000</v>
       </c>
@@ -1050,23 +1050,23 @@
     </row>
     <row r="9" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="19" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="19" t="s">
+      <c r="F10" s="23"/>
+      <c r="G10" s="22" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="20"/>
-      <c r="I10" s="22"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="20" t="s">
         <v>3</v>
       </c>
@@ -1074,55 +1074,55 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="20"/>
-      <c r="O10" s="22"/>
+      <c r="O10" s="21"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="24" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="24" t="s">
+      <c r="K11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="24" t="s">
+      <c r="L11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="24" t="s">
+      <c r="M11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="26" t="s">
+      <c r="O11" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="2">
         <v>100</v>
       </c>
@@ -1170,7 +1170,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="2">
         <v>1000</v>
       </c>
@@ -1218,7 +1218,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="2">
         <v>5000</v>
       </c>
@@ -1266,7 +1266,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="2">
         <v>10000</v>
       </c>
@@ -1314,7 +1314,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="18"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="9">
         <v>15000</v>
       </c>
@@ -1363,23 +1363,23 @@
     </row>
     <row r="17" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="19" t="s">
+      <c r="A18" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="19" t="s">
+      <c r="D18" s="23"/>
+      <c r="E18" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="19" t="s">
+      <c r="F18" s="23"/>
+      <c r="G18" s="22" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="20"/>
-      <c r="I18" s="22"/>
+      <c r="I18" s="21"/>
       <c r="J18" s="20" t="s">
         <v>3</v>
       </c>
@@ -1387,55 +1387,55 @@
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
       <c r="N18" s="20"/>
-      <c r="O18" s="22"/>
+      <c r="O18" s="21"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="A19" s="25"/>
+      <c r="B19" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K19" s="24" t="s">
+      <c r="K19" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="L19" s="24" t="s">
+      <c r="L19" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="24" t="s">
+      <c r="M19" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="N19" s="24" t="s">
+      <c r="N19" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="O19" s="26" t="s">
+      <c r="O19" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="2">
         <v>100</v>
       </c>
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="2">
         <v>1000</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>14.992503748125937</v>
       </c>
       <c r="I21" s="7">
-        <f t="shared" ref="I21:I24" si="8">O21/(J21+K21)</f>
+        <f t="shared" ref="I21:I23" si="8">O21/(J21+K21)</f>
         <v>0.24390243902439024</v>
       </c>
       <c r="J21" s="3">
@@ -1531,7 +1531,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="2">
         <v>5000</v>
       </c>
@@ -1579,7 +1579,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="2">
         <v>10000</v>
       </c>
@@ -1627,7 +1627,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="18"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="9">
         <v>15000</v>
       </c>
@@ -1676,23 +1676,23 @@
     </row>
     <row r="25" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="19" t="s">
+      <c r="A26" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="19" t="s">
+      <c r="D26" s="23"/>
+      <c r="E26" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="19" t="s">
+      <c r="F26" s="23"/>
+      <c r="G26" s="22" t="s">
         <v>9</v>
       </c>
       <c r="H26" s="20"/>
-      <c r="I26" s="22"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="20" t="s">
         <v>3</v>
       </c>
@@ -1700,55 +1700,55 @@
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
-      <c r="O26" s="22"/>
+      <c r="O26" s="21"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="24" t="s">
+      <c r="A27" s="25"/>
+      <c r="B27" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="23" t="s">
+      <c r="G27" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="H27" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I27" s="26" t="s">
+      <c r="I27" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J27" s="24" t="s">
+      <c r="J27" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K27" s="24" t="s">
+      <c r="K27" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="L27" s="24" t="s">
+      <c r="L27" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="M27" s="24" t="s">
+      <c r="M27" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="N27" s="24" t="s">
+      <c r="N27" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="O27" s="26" t="s">
+      <c r="O27" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="2">
         <v>100</v>
       </c>
@@ -1796,7 +1796,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="2">
         <v>1000</v>
       </c>
@@ -1844,7 +1844,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="2">
         <v>5000</v>
       </c>
@@ -1892,7 +1892,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="2">
         <v>10000</v>
       </c>
@@ -1940,7 +1940,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="18"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="9">
         <v>15000</v>
       </c>
@@ -1989,18 +1989,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="J18:O18"/>
-    <mergeCell ref="J26:O26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="B2:D2"/>
@@ -2009,6 +1997,18 @@
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="J10:O10"/>
     <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A26:A32"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="J26:O26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>